<commit_message>
integrate jquery ui and jquery theme into project.
</commit_message>
<xml_diff>
--- a/Documents/DailyPlan.xlsx
+++ b/Documents/DailyPlan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>20:30-22:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -83,6 +83,110 @@
   </si>
   <si>
     <t>1h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jquery</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ui</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>theme</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>css framework</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>layout framework</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>21:00-23:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>study and integrate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Datepicker</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Autocomplete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Progressbar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dialog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>model dialog, model form</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tabs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ToggleClass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Effect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Position</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>23:00-23:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.5h</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -504,14 +608,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E12:L20"/>
+  <dimension ref="E12:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
+    <col min="6" max="6" width="5.75" customWidth="1"/>
     <col min="8" max="9" width="13.75" customWidth="1"/>
   </cols>
   <sheetData>
@@ -562,6 +667,119 @@
         <v>16</v>
       </c>
     </row>
+    <row r="23" spans="5:12" x14ac:dyDescent="0.15">
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="F23" t="s">
+        <v>30</v>
+      </c>
+      <c r="J23" t="s">
+        <v>27</v>
+      </c>
+      <c r="L23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="5:12" x14ac:dyDescent="0.15">
+      <c r="J24" t="s">
+        <v>41</v>
+      </c>
+      <c r="L24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="5:12" x14ac:dyDescent="0.15">
+      <c r="F25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" t="s">
+        <v>17</v>
+      </c>
+      <c r="L25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="5:12" x14ac:dyDescent="0.15">
+      <c r="F26" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="5:12" x14ac:dyDescent="0.15">
+      <c r="H27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="5:12" x14ac:dyDescent="0.15">
+      <c r="H28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="5:12" x14ac:dyDescent="0.15">
+      <c r="H29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="5:12" x14ac:dyDescent="0.15">
+      <c r="H30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="5:12" x14ac:dyDescent="0.15">
+      <c r="H31" t="s">
+        <v>35</v>
+      </c>
+      <c r="I31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="5:12" x14ac:dyDescent="0.15">
+      <c r="H32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="6:8" x14ac:dyDescent="0.15">
+      <c r="H33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="6:8" x14ac:dyDescent="0.15">
+      <c r="H34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="6:8" x14ac:dyDescent="0.15">
+      <c r="H35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="6:8" x14ac:dyDescent="0.15">
+      <c r="F37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G37" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="6:8" x14ac:dyDescent="0.15">
+      <c r="F38" t="s">
+        <v>23</v>
+      </c>
+      <c r="G38" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="6:8" x14ac:dyDescent="0.15">
+      <c r="F39" t="s">
+        <v>25</v>
+      </c>
+      <c r="G39" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
jqgrid integration; change js plugins file structure.
</commit_message>
<xml_diff>
--- a/Documents/DailyPlan.xlsx
+++ b/Documents/DailyPlan.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="20120806" sheetId="9" r:id="rId1"/>
     <sheet name="20120807" sheetId="10" r:id="rId2"/>
     <sheet name="20120808" sheetId="11" r:id="rId3"/>
+    <sheet name="20120809" sheetId="12" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>20:30-22:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -187,6 +188,26 @@
   </si>
   <si>
     <t>2.5h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>study jquery grid plugin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6:00-8:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8:00-8:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.5h</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -610,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E12:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -784,4 +805,43 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E12:L13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="12" spans="5:12" x14ac:dyDescent="0.15">
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>43</v>
+      </c>
+      <c r="J12" t="s">
+        <v>44</v>
+      </c>
+      <c r="L12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="5:12" x14ac:dyDescent="0.15">
+      <c r="J13" t="s">
+        <v>46</v>
+      </c>
+      <c r="L13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
setup basic system layout
</commit_message>
<xml_diff>
--- a/Documents/DailyPlan.xlsx
+++ b/Documents/DailyPlan.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="20120806" sheetId="9" r:id="rId1"/>
     <sheet name="20120807" sheetId="10" r:id="rId2"/>
     <sheet name="20120808" sheetId="11" r:id="rId3"/>
     <sheet name="20120809" sheetId="12" r:id="rId4"/>
+    <sheet name="20120810" sheetId="13" r:id="rId5"/>
+    <sheet name="20120811" sheetId="14" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
   <si>
     <t>20:30-22:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -220,6 +222,30 @@
   </si>
   <si>
     <t>2h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7:00-8:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>finish basic layout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>study jquery layout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15:15-16:15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16:15-17:15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1h</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -251,7 +277,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -413,11 +439,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -434,6 +475,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -812,7 +854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E12:L39"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
@@ -992,8 +1034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E12:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16:L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1087,4 +1129,150 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="F13:L24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="13" spans="6:12" x14ac:dyDescent="0.15">
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>48</v>
+      </c>
+      <c r="J13" t="s">
+        <v>51</v>
+      </c>
+      <c r="L13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="6:12" x14ac:dyDescent="0.15">
+      <c r="G15" s="6"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="8"/>
+    </row>
+    <row r="16" spans="6:12" x14ac:dyDescent="0.15">
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+    </row>
+    <row r="17" spans="7:11" x14ac:dyDescent="0.15">
+      <c r="G17" s="3"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="11"/>
+    </row>
+    <row r="18" spans="7:11" x14ac:dyDescent="0.15">
+      <c r="G18" s="4"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="13"/>
+    </row>
+    <row r="19" spans="7:11" x14ac:dyDescent="0.15">
+      <c r="G19" s="4"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="13"/>
+    </row>
+    <row r="20" spans="7:11" x14ac:dyDescent="0.15">
+      <c r="G20" s="4"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="13"/>
+    </row>
+    <row r="21" spans="7:11" x14ac:dyDescent="0.15">
+      <c r="G21" s="4"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="13"/>
+    </row>
+    <row r="22" spans="7:11" x14ac:dyDescent="0.15">
+      <c r="G22" s="4"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="13"/>
+    </row>
+    <row r="23" spans="7:11" x14ac:dyDescent="0.15">
+      <c r="G23" s="4"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="13"/>
+    </row>
+    <row r="24" spans="7:11" x14ac:dyDescent="0.15">
+      <c r="G24" s="5"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="15"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="F11:L14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="11" spans="6:12" x14ac:dyDescent="0.15">
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>53</v>
+      </c>
+      <c r="J11" t="s">
+        <v>54</v>
+      </c>
+      <c r="L11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="6:12" x14ac:dyDescent="0.15">
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>52</v>
+      </c>
+      <c r="J14" t="s">
+        <v>55</v>
+      </c>
+      <c r="L14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
set up basic left menu.
</commit_message>
<xml_diff>
--- a/Documents/DailyPlan.xlsx
+++ b/Documents/DailyPlan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="20120806" sheetId="9" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="60">
   <si>
     <t>20:30-22:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -246,6 +246,18 @@
   </si>
   <si>
     <t>1h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>search jquery menu and tree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>22:00-23:40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.5h</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1133,10 +1145,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F13:L24"/>
+  <dimension ref="F13:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15:K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1154,76 +1166,6 @@
       <c r="L13" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="6:12" x14ac:dyDescent="0.15">
-      <c r="G15" s="6"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="8"/>
-    </row>
-    <row r="16" spans="6:12" x14ac:dyDescent="0.15">
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-    </row>
-    <row r="17" spans="7:11" x14ac:dyDescent="0.15">
-      <c r="G17" s="3"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="11"/>
-    </row>
-    <row r="18" spans="7:11" x14ac:dyDescent="0.15">
-      <c r="G18" s="4"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="13"/>
-    </row>
-    <row r="19" spans="7:11" x14ac:dyDescent="0.15">
-      <c r="G19" s="4"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="13"/>
-    </row>
-    <row r="20" spans="7:11" x14ac:dyDescent="0.15">
-      <c r="G20" s="4"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="13"/>
-    </row>
-    <row r="21" spans="7:11" x14ac:dyDescent="0.15">
-      <c r="G21" s="4"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="13"/>
-    </row>
-    <row r="22" spans="7:11" x14ac:dyDescent="0.15">
-      <c r="G22" s="4"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="13"/>
-    </row>
-    <row r="23" spans="7:11" x14ac:dyDescent="0.15">
-      <c r="G23" s="4"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="13"/>
-    </row>
-    <row r="24" spans="7:11" x14ac:dyDescent="0.15">
-      <c r="G24" s="5"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1234,41 +1176,135 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F11:L14"/>
+  <dimension ref="F11:M28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="11" spans="6:12" x14ac:dyDescent="0.15">
+    <row r="11" spans="6:13" x14ac:dyDescent="0.15">
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11" t="s">
         <v>53</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>54</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="6:12" x14ac:dyDescent="0.15">
+    <row r="14" spans="6:13" x14ac:dyDescent="0.15">
       <c r="F14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G14" t="s">
         <v>52</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>55</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>56</v>
       </c>
+    </row>
+    <row r="16" spans="6:13" x14ac:dyDescent="0.15">
+      <c r="F16">
+        <v>3</v>
+      </c>
+      <c r="G16" t="s">
+        <v>57</v>
+      </c>
+      <c r="K16" t="s">
+        <v>58</v>
+      </c>
+      <c r="M16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="7:12" x14ac:dyDescent="0.15">
+      <c r="G19" s="6"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="8"/>
+    </row>
+    <row r="20" spans="7:12" x14ac:dyDescent="0.15">
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+    </row>
+    <row r="21" spans="7:12" x14ac:dyDescent="0.15">
+      <c r="G21" s="3"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="11"/>
+    </row>
+    <row r="22" spans="7:12" x14ac:dyDescent="0.15">
+      <c r="G22" s="4"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="13"/>
+    </row>
+    <row r="23" spans="7:12" x14ac:dyDescent="0.15">
+      <c r="G23" s="4"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="13"/>
+    </row>
+    <row r="24" spans="7:12" x14ac:dyDescent="0.15">
+      <c r="G24" s="4"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="13"/>
+    </row>
+    <row r="25" spans="7:12" x14ac:dyDescent="0.15">
+      <c r="G25" s="4"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="13"/>
+    </row>
+    <row r="26" spans="7:12" x14ac:dyDescent="0.15">
+      <c r="G26" s="4"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="13"/>
+    </row>
+    <row r="27" spans="7:12" x14ac:dyDescent="0.15">
+      <c r="G27" s="4"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="13"/>
+    </row>
+    <row r="28" spans="7:12" x14ac:dyDescent="0.15">
+      <c r="G28" s="5"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
use JAXB to parse menus.xml dynamically.
</commit_message>
<xml_diff>
--- a/Documents/DailyPlan.xlsx
+++ b/Documents/DailyPlan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="20120806" sheetId="9" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="20120809" sheetId="12" r:id="rId4"/>
     <sheet name="20120810" sheetId="13" r:id="rId5"/>
     <sheet name="20120811" sheetId="14" r:id="rId6"/>
+    <sheet name="20120812" sheetId="15" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="69">
   <si>
     <t>20:30-22:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -258,6 +259,42 @@
   </si>
   <si>
     <t>1.5h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create system menu base on xml</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>study java manipulate xml</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9:30-10:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10:30-11:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>design menu structure and parse menu.xml</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jaxb import?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>menus.xml location?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>resource directory function?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1178,8 +1215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F11:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1311,4 +1348,72 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E10:M18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="10" spans="5:13" x14ac:dyDescent="0.15">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>61</v>
+      </c>
+      <c r="K10" t="s">
+        <v>62</v>
+      </c>
+      <c r="M10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="5:13" x14ac:dyDescent="0.15">
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>65</v>
+      </c>
+      <c r="K12" t="s">
+        <v>64</v>
+      </c>
+      <c r="M12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="5:13" x14ac:dyDescent="0.15">
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="5:13" x14ac:dyDescent="0.15">
+      <c r="F16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
auto generate system menus base on menus.xml.
</commit_message>
<xml_diff>
--- a/Documents/DailyPlan.xlsx
+++ b/Documents/DailyPlan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="20120806" sheetId="9" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="20120810" sheetId="13" r:id="rId5"/>
     <sheet name="20120811" sheetId="14" r:id="rId6"/>
     <sheet name="20120812" sheetId="15" r:id="rId7"/>
+    <sheet name="20120813" sheetId="16" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="72">
   <si>
     <t>20:30-22:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -295,6 +296,18 @@
   </si>
   <si>
     <t>resource directory function?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>auto generate system menus base on menus.xml</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10:30-12:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.5h</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -903,7 +916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E12:L39"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
@@ -1083,7 +1096,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E12:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16:L16"/>
     </sheetView>
   </sheetViews>
@@ -1184,7 +1197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F13:L13"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15:K24"/>
     </sheetView>
   </sheetViews>
@@ -1216,7 +1229,7 @@
   <dimension ref="F11:M28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1352,10 +1365,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E10:M18"/>
+  <dimension ref="E10:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1388,27 +1401,74 @@
         <v>16</v>
       </c>
     </row>
+    <row r="13" spans="5:13" x14ac:dyDescent="0.15">
+      <c r="K13" t="s">
+        <v>54</v>
+      </c>
+      <c r="M13" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="14" spans="5:13" x14ac:dyDescent="0.15">
-      <c r="E14">
+      <c r="K14" t="s">
+        <v>55</v>
+      </c>
+      <c r="M14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="5:13" x14ac:dyDescent="0.15">
+      <c r="E16">
         <v>3</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F16" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="5:13" x14ac:dyDescent="0.15">
-      <c r="F16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.15">
-      <c r="F17" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F20" t="s">
         <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E12:N12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="12" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>69</v>
+      </c>
+      <c r="L12" t="s">
+        <v>70</v>
+      </c>
+      <c r="N12" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
study include,jsp:include and optimize header.jsp. use errorPage attribute for error handling.
</commit_message>
<xml_diff>
--- a/Documents/DailyPlan.xlsx
+++ b/Documents/DailyPlan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="20120806" sheetId="9" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="20120811" sheetId="14" r:id="rId6"/>
     <sheet name="20120812" sheetId="15" r:id="rId7"/>
     <sheet name="20120813" sheetId="16" r:id="rId8"/>
+    <sheet name="20120814" sheetId="17" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="78">
   <si>
     <t>20:30-22:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -308,6 +309,30 @@
   </si>
   <si>
     <t>1.5h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>study SSH integration</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>21:30-23:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.5h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6:45-7:45</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6:45-8:45</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1449,10 +1474,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E12:N12"/>
+  <dimension ref="E12:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14:N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1471,6 +1496,59 @@
         <v>71</v>
       </c>
     </row>
+    <row r="14" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>72</v>
+      </c>
+      <c r="L14" t="s">
+        <v>73</v>
+      </c>
+      <c r="N14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E13:L14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="13" spans="5:12" x14ac:dyDescent="0.15">
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>72</v>
+      </c>
+      <c r="J13" t="s">
+        <v>75</v>
+      </c>
+      <c r="L13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="5:12" x14ac:dyDescent="0.15">
+      <c r="J14" t="s">
+        <v>77</v>
+      </c>
+      <c r="L14" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
set error global-forwards and optimize error.jsp.
</commit_message>
<xml_diff>
--- a/Documents/DailyPlan.xlsx
+++ b/Documents/DailyPlan.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="85">
   <si>
     <t>20:30-22:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -353,6 +353,14 @@
   </si>
   <si>
     <t>13:30-14:40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14:40-15:40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16:00-17:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1539,10 +1547,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E13:L18"/>
+  <dimension ref="E13:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1593,6 +1601,22 @@
         <v>81</v>
       </c>
     </row>
+    <row r="19" spans="10:12" x14ac:dyDescent="0.15">
+      <c r="J19" t="s">
+        <v>83</v>
+      </c>
+      <c r="L19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="10:12" x14ac:dyDescent="0.15">
+      <c r="J20" t="s">
+        <v>84</v>
+      </c>
+      <c r="L20" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
test transaction management with BeanNameAutoProxyCreator.
</commit_message>
<xml_diff>
--- a/Documents/DailyPlan.xlsx
+++ b/Documents/DailyPlan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" firstSheet="4" activeTab="12"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" firstSheet="5" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="20120806" sheetId="9" r:id="rId1"/>
@@ -20,13 +20,14 @@
     <sheet name="20120821" sheetId="19" r:id="rId11"/>
     <sheet name="20120823" sheetId="20" r:id="rId12"/>
     <sheet name="20120825" sheetId="21" r:id="rId13"/>
+    <sheet name="20120827" sheetId="22" r:id="rId14"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="114">
   <si>
     <t>20:30-22:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -469,6 +470,18 @@
   </si>
   <si>
     <t>9:30-11:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add transaction control</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9:10-10:10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1h</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1218,8 +1231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F12:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1236,6 +1249,37 @@
       </c>
       <c r="L12" t="s">
         <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E13:L13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="13" spans="5:12" x14ac:dyDescent="0.15">
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>111</v>
+      </c>
+      <c r="J13" t="s">
+        <v>112</v>
+      </c>
+      <c r="L13" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
design DAO interface and DAO implement class.
</commit_message>
<xml_diff>
--- a/Documents/DailyPlan.xlsx
+++ b/Documents/DailyPlan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" firstSheet="5" activeTab="13"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" firstSheet="9" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="20120806" sheetId="9" r:id="rId1"/>
@@ -21,13 +21,17 @@
     <sheet name="20120823" sheetId="20" r:id="rId12"/>
     <sheet name="20120825" sheetId="21" r:id="rId13"/>
     <sheet name="20120827" sheetId="22" r:id="rId14"/>
+    <sheet name="20120902" sheetId="23" r:id="rId15"/>
+    <sheet name="20120903" sheetId="24" r:id="rId16"/>
+    <sheet name="20120904" sheetId="25" r:id="rId17"/>
+    <sheet name="20120905" sheetId="26" r:id="rId18"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="129">
   <si>
     <t>20:30-22:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -478,6 +482,66 @@
   </si>
   <si>
     <t>9:10-10:10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10:10-10:40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.5h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>read SSH book</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11:30-12:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20:20-21:20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>read SSH book</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8:40-9:40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>optimizie lifeRudder framework</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15:30-16:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10:30-11:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12:50-13:50</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1260,10 +1324,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E13:L13"/>
+  <dimension ref="E13:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1280,6 +1344,160 @@
       </c>
       <c r="L13" t="s">
         <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="5:12" x14ac:dyDescent="0.15">
+      <c r="J14" t="s">
+        <v>114</v>
+      </c>
+      <c r="L14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="5:12" x14ac:dyDescent="0.15">
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16" t="s">
+        <v>116</v>
+      </c>
+      <c r="J16" t="s">
+        <v>117</v>
+      </c>
+      <c r="L16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="F14:K14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14:K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="14" spans="6:11" x14ac:dyDescent="0.15">
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>116</v>
+      </c>
+      <c r="I14" t="s">
+        <v>119</v>
+      </c>
+      <c r="K14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="F14:K14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="14" spans="6:11" x14ac:dyDescent="0.15">
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>121</v>
+      </c>
+      <c r="I14" t="s">
+        <v>122</v>
+      </c>
+      <c r="K14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="F14:M14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14:M14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="14" spans="6:13" x14ac:dyDescent="0.15">
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>123</v>
+      </c>
+      <c r="K14" t="s">
+        <v>124</v>
+      </c>
+      <c r="M14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E13:L15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="13" spans="5:12" x14ac:dyDescent="0.15">
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>123</v>
+      </c>
+      <c r="J13" t="s">
+        <v>126</v>
+      </c>
+      <c r="L13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="5:12" x14ac:dyDescent="0.15">
+      <c r="J15" t="s">
+        <v>127</v>
+      </c>
+      <c r="L15" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
design bo layer and add transaction control to bo classes with BeanNameAutoProxyCreator instead of DefaultAdvisorAutoProxyCreator.
</commit_message>
<xml_diff>
--- a/Documents/DailyPlan.xlsx
+++ b/Documents/DailyPlan.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="131">
   <si>
     <t>20:30-22:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -541,7 +541,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>1h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>12:50-13:50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13:50-14:50</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1470,10 +1478,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E13:L15"/>
+  <dimension ref="E13:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1494,10 +1502,18 @@
     </row>
     <row r="15" spans="5:12" x14ac:dyDescent="0.15">
       <c r="J15" t="s">
+        <v>128</v>
+      </c>
+      <c r="L15" t="s">
         <v>127</v>
       </c>
-      <c r="L15" t="s">
-        <v>128</v>
+    </row>
+    <row r="17" spans="10:12" x14ac:dyDescent="0.15">
+      <c r="J17" t="s">
+        <v>129</v>
+      </c>
+      <c r="L17" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix Chinese messy code issue by extending ActionServlet instead of Filter.
</commit_message>
<xml_diff>
--- a/Documents/DailyPlan.xlsx
+++ b/Documents/DailyPlan.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="133">
   <si>
     <t>20:30-22:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -549,7 +549,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>1h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>13:50-14:50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14:50-15:50</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1478,10 +1486,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E13:L17"/>
+  <dimension ref="E13:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1510,10 +1518,18 @@
     </row>
     <row r="17" spans="10:12" x14ac:dyDescent="0.15">
       <c r="J17" t="s">
+        <v>130</v>
+      </c>
+      <c r="L17" t="s">
         <v>129</v>
       </c>
-      <c r="L17" t="s">
-        <v>130</v>
+    </row>
+    <row r="19" spans="10:12" x14ac:dyDescent="0.15">
+      <c r="J19" t="s">
+        <v>131</v>
+      </c>
+      <c r="L19" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update jquery related files.
</commit_message>
<xml_diff>
--- a/Documents/DailyPlan.xlsx
+++ b/Documents/DailyPlan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" firstSheet="9" activeTab="17"/>
+    <workbookView xWindow="240" yWindow="255" windowWidth="14805" windowHeight="7860" firstSheet="13" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="20120806" sheetId="9" r:id="rId1"/>
@@ -25,13 +25,16 @@
     <sheet name="20120903" sheetId="24" r:id="rId16"/>
     <sheet name="20120904" sheetId="25" r:id="rId17"/>
     <sheet name="20120905" sheetId="26" r:id="rId18"/>
+    <sheet name="20120906" sheetId="27" r:id="rId19"/>
+    <sheet name="20120907" sheetId="28" r:id="rId20"/>
+    <sheet name="20120917" sheetId="29" r:id="rId21"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="158">
   <si>
     <t>20:30-22:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -562,6 +565,106 @@
   </si>
   <si>
     <t>1h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jquery-ui</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jqgrid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jquery</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jquery-layout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tabs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jquery-ui-theme</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20:10-21:10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>study css</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>study jquery</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>study jquery ui</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>study jquery ui theme</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>study CSS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9:30-10:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.5h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11:00-11:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>study jQurey</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14:30-15:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.5h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>study jquery ui</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>21:00-22:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>22:45-23:45</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update jquery plugin files</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1488,7 +1591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E13:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
@@ -1530,6 +1633,80 @@
       </c>
       <c r="L19" t="s">
         <v>132</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="F12:K21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="7" max="7" width="7.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="12" spans="6:11" x14ac:dyDescent="0.15">
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>137</v>
+      </c>
+      <c r="I12" t="s">
+        <v>141</v>
+      </c>
+      <c r="K12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="6:11" x14ac:dyDescent="0.15">
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="6:11" x14ac:dyDescent="0.15">
+      <c r="G15" t="s">
+        <v>139</v>
+      </c>
+      <c r="H15" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="6:7" x14ac:dyDescent="0.15">
+      <c r="F17">
+        <v>3</v>
+      </c>
+      <c r="G17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="6:7" x14ac:dyDescent="0.15">
+      <c r="F19">
+        <v>4</v>
+      </c>
+      <c r="G19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="6:7" x14ac:dyDescent="0.15">
+      <c r="F21">
+        <v>5</v>
+      </c>
+      <c r="G21" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1570,11 +1747,147 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="F11:L17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="11" spans="6:12" x14ac:dyDescent="0.15">
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>142</v>
+      </c>
+      <c r="J11" t="s">
+        <v>62</v>
+      </c>
+      <c r="L11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="6:12" x14ac:dyDescent="0.15">
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="6:12" x14ac:dyDescent="0.15">
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="G15" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="6:7" x14ac:dyDescent="0.15">
+      <c r="F17">
+        <v>4</v>
+      </c>
+      <c r="G17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E12:L20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="12" spans="5:12" x14ac:dyDescent="0.15">
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>147</v>
+      </c>
+      <c r="J12" t="s">
+        <v>148</v>
+      </c>
+      <c r="L12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="5:12" x14ac:dyDescent="0.15">
+      <c r="J13" t="s">
+        <v>150</v>
+      </c>
+      <c r="L13" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="5:12" x14ac:dyDescent="0.15">
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>151</v>
+      </c>
+      <c r="J15" t="s">
+        <v>152</v>
+      </c>
+      <c r="L15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" spans="5:12" x14ac:dyDescent="0.15">
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18" t="s">
+        <v>154</v>
+      </c>
+      <c r="J18" t="s">
+        <v>155</v>
+      </c>
+      <c r="L18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="5:12" x14ac:dyDescent="0.15">
+      <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="F20" t="s">
+        <v>157</v>
+      </c>
+      <c r="J20" t="s">
+        <v>156</v>
+      </c>
+      <c r="L20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E12:L39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update style of login.jsp and main_frame.jsp.
</commit_message>
<xml_diff>
--- a/Documents/DailyPlan.xlsx
+++ b/Documents/DailyPlan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="255" windowWidth="14805" windowHeight="7860" firstSheet="13" activeTab="20"/>
+    <workbookView xWindow="240" yWindow="255" windowWidth="14805" windowHeight="7860" firstSheet="13" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="20120806" sheetId="9" r:id="rId1"/>
@@ -28,13 +28,14 @@
     <sheet name="20120906" sheetId="27" r:id="rId19"/>
     <sheet name="20120907" sheetId="28" r:id="rId20"/>
     <sheet name="20120917" sheetId="29" r:id="rId21"/>
+    <sheet name="20120918" sheetId="30" r:id="rId22"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="167">
   <si>
     <t>20:30-22:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -665,6 +666,42 @@
   </si>
   <si>
     <t>update jquery plugin files</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI update</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14:00-16:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>menu tree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>header</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>form</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>list</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1806,8 +1843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E12:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1874,6 +1911,80 @@
       </c>
       <c r="L20" t="s">
         <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="F14:K19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="7" max="7" width="6.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="14" spans="6:11" x14ac:dyDescent="0.15">
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>158</v>
+      </c>
+      <c r="I14" t="s">
+        <v>159</v>
+      </c>
+      <c r="K14" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15" spans="6:11" x14ac:dyDescent="0.15">
+      <c r="G15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="6:11" x14ac:dyDescent="0.15">
+      <c r="G16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.15">
+      <c r="G17" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="7:8" x14ac:dyDescent="0.15">
+      <c r="G18" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="7:8" x14ac:dyDescent="0.15">
+      <c r="G19" t="s">
+        <v>165</v>
+      </c>
+      <c r="H19" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix issue: include js after <base href="<%=basePath%>">.
</commit_message>
<xml_diff>
--- a/Documents/DailyPlan.xlsx
+++ b/Documents/DailyPlan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="255" windowWidth="14805" windowHeight="7860" firstSheet="13" activeTab="21"/>
+    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830" firstSheet="16" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="20120806" sheetId="9" r:id="rId1"/>
@@ -29,13 +29,16 @@
     <sheet name="20120907" sheetId="28" r:id="rId20"/>
     <sheet name="20120917" sheetId="29" r:id="rId21"/>
     <sheet name="20120918" sheetId="30" r:id="rId22"/>
+    <sheet name="20120921" sheetId="31" r:id="rId23"/>
+    <sheet name="20120922" sheetId="32" r:id="rId24"/>
+    <sheet name="20120923" sheetId="33" r:id="rId25"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="180">
   <si>
     <t>20:30-22:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -681,27 +684,79 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>form</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20:00-21:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.5h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>header</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>menu tree</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>header</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>button</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>form</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>e</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>list</t>
+    <t>error hint solution</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11:30-12:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.5h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13:30-14:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JS debug tool?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10:00-11:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11:00-12:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>22:00-23:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1922,10 +1977,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F14:K19"/>
+  <dimension ref="F14:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1948,43 +2003,176 @@
       </c>
     </row>
     <row r="15" spans="6:11" x14ac:dyDescent="0.15">
-      <c r="G15" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" t="s">
-        <v>161</v>
+      <c r="I15" t="s">
+        <v>166</v>
+      </c>
+      <c r="K15" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="6:11" x14ac:dyDescent="0.15">
       <c r="G16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H16" t="s">
-        <v>162</v>
+        <v>169</v>
+      </c>
+      <c r="J16" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="7:8" x14ac:dyDescent="0.15">
       <c r="G17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H17" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="7:8" x14ac:dyDescent="0.15">
       <c r="G18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H18" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="7:8" x14ac:dyDescent="0.15">
       <c r="G19" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" t="s">
         <v>165</v>
       </c>
-      <c r="H19" t="s">
-        <v>166</v>
+    </row>
+    <row r="20" spans="7:8" x14ac:dyDescent="0.15">
+      <c r="G20" t="s">
+        <v>162</v>
+      </c>
+      <c r="H20" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E13:K17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13:K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="13" spans="5:11" x14ac:dyDescent="0.15">
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>170</v>
+      </c>
+      <c r="I13" t="s">
+        <v>172</v>
+      </c>
+      <c r="K13" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="15" spans="5:11" x14ac:dyDescent="0.15">
+      <c r="I15" t="s">
+        <v>174</v>
+      </c>
+      <c r="K15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.15">
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="F11:L13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13:L13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="11" spans="6:12" x14ac:dyDescent="0.15">
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>175</v>
+      </c>
+      <c r="J11" t="s">
+        <v>176</v>
+      </c>
+      <c r="L11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="13" spans="6:12" x14ac:dyDescent="0.15">
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>170</v>
+      </c>
+      <c r="J13" t="s">
+        <v>178</v>
+      </c>
+      <c r="L13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="F12:L12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="12" spans="6:12" x14ac:dyDescent="0.15">
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>170</v>
+      </c>
+      <c r="J12" t="s">
+        <v>179</v>
+      </c>
+      <c r="L12" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
enhance paging feature,support custom format for query result list.
</commit_message>
<xml_diff>
--- a/Documents/DailyPlan.xlsx
+++ b/Documents/DailyPlan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830" firstSheet="16" activeTab="24"/>
+    <workbookView xWindow="240" yWindow="315" windowWidth="14805" windowHeight="7800" firstSheet="19" activeTab="27"/>
   </bookViews>
   <sheets>
     <sheet name="20120806" sheetId="9" r:id="rId1"/>
@@ -32,13 +32,16 @@
     <sheet name="20120921" sheetId="31" r:id="rId23"/>
     <sheet name="20120922" sheetId="32" r:id="rId24"/>
     <sheet name="20120923" sheetId="33" r:id="rId25"/>
+    <sheet name="20120924" sheetId="34" r:id="rId26"/>
+    <sheet name="20121114" sheetId="35" r:id="rId27"/>
+    <sheet name="20121115" sheetId="36" r:id="rId28"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="204">
   <si>
     <t>20:30-22:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -758,6 +761,95 @@
   <si>
     <t>22:00-23:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hint display only when submit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>one hint one time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>don't need dynamical hint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hint:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hint css style</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>submit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>study jquery-validate's usage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lifeRudder update</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10:00-11:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.5h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>change mysql to HSQLDB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JDBC enhancement</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13:30-15:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lifeRudder update</t>
+  </si>
+  <si>
+    <t>13:30-15:00</t>
+  </si>
+  <si>
+    <t>1.5h</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>change mysql to HSQLDB</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>JDBC enhancement</t>
   </si>
 </sst>
 </file>
@@ -2155,8 +2247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F12:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2173,6 +2265,272 @@
       </c>
       <c r="L12" t="s">
         <v>177</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="F13:L34"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="6" max="6" width="6.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="13" spans="6:12" x14ac:dyDescent="0.15">
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>170</v>
+      </c>
+      <c r="J13" t="s">
+        <v>178</v>
+      </c>
+      <c r="L13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="6:12" x14ac:dyDescent="0.15">
+      <c r="F14" t="s">
+        <v>186</v>
+      </c>
+      <c r="G14" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="15" spans="6:12" x14ac:dyDescent="0.15">
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="16" spans="6:12" x14ac:dyDescent="0.15">
+      <c r="F16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="17" spans="6:10" x14ac:dyDescent="0.15">
+      <c r="F17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="18" spans="6:10" x14ac:dyDescent="0.15">
+      <c r="F18" t="s">
+        <v>162</v>
+      </c>
+      <c r="G18" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="21" spans="6:10" x14ac:dyDescent="0.15">
+      <c r="G21" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="6:10" x14ac:dyDescent="0.15">
+      <c r="G22" s="12"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="13"/>
+    </row>
+    <row r="23" spans="6:10" x14ac:dyDescent="0.15">
+      <c r="G23" s="12"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="16"/>
+    </row>
+    <row r="24" spans="6:10" x14ac:dyDescent="0.15">
+      <c r="G24" s="12"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="13"/>
+    </row>
+    <row r="25" spans="6:10" x14ac:dyDescent="0.15">
+      <c r="G25" s="12"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="16"/>
+    </row>
+    <row r="26" spans="6:10" x14ac:dyDescent="0.15">
+      <c r="G26" s="12"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="13"/>
+    </row>
+    <row r="27" spans="6:10" x14ac:dyDescent="0.15">
+      <c r="G27" s="12"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="13"/>
+    </row>
+    <row r="28" spans="6:10" x14ac:dyDescent="0.15">
+      <c r="G28" s="12"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="13"/>
+    </row>
+    <row r="29" spans="6:10" x14ac:dyDescent="0.15">
+      <c r="G29" s="12"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="13"/>
+    </row>
+    <row r="30" spans="6:10" x14ac:dyDescent="0.15">
+      <c r="G30" s="12"/>
+      <c r="H30" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="I30" s="1"/>
+      <c r="J30" s="13"/>
+    </row>
+    <row r="31" spans="6:10" x14ac:dyDescent="0.15">
+      <c r="G31" s="12"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="13"/>
+    </row>
+    <row r="32" spans="6:10" x14ac:dyDescent="0.15">
+      <c r="G32" s="12"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="13"/>
+    </row>
+    <row r="33" spans="7:10" x14ac:dyDescent="0.15">
+      <c r="G33" s="12"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="13"/>
+    </row>
+    <row r="34" spans="7:10" x14ac:dyDescent="0.15">
+      <c r="G34" s="14"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="15"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="F11:L15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="11" spans="6:12" x14ac:dyDescent="0.15">
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>188</v>
+      </c>
+      <c r="J11" t="s">
+        <v>189</v>
+      </c>
+      <c r="L11" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="12" spans="6:12" x14ac:dyDescent="0.15">
+      <c r="G12" t="s">
+        <v>191</v>
+      </c>
+      <c r="H12" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="13" spans="6:12" x14ac:dyDescent="0.15">
+      <c r="G13" t="s">
+        <v>193</v>
+      </c>
+      <c r="H13" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="15" spans="6:12" x14ac:dyDescent="0.15">
+      <c r="J15" t="s">
+        <v>195</v>
+      </c>
+      <c r="L15" t="s">
+        <v>196</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="F10:L12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="7" max="7" width="6.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="10" spans="6:12" x14ac:dyDescent="0.15">
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>197</v>
+      </c>
+      <c r="J10" t="s">
+        <v>198</v>
+      </c>
+      <c r="L10" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="11" spans="6:12" x14ac:dyDescent="0.15">
+      <c r="G11" t="s">
+        <v>200</v>
+      </c>
+      <c r="H11" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="12" spans="6:12" x14ac:dyDescent="0.15">
+      <c r="G12" t="s">
+        <v>202</v>
+      </c>
+      <c r="H12" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change database from mysql to hsqldb.
</commit_message>
<xml_diff>
--- a/Documents/DailyPlan.xlsx
+++ b/Documents/DailyPlan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="315" windowWidth="14805" windowHeight="7800" firstSheet="19" activeTab="27"/>
+    <workbookView xWindow="240" yWindow="315" windowWidth="14805" windowHeight="7800" firstSheet="20" activeTab="28"/>
   </bookViews>
   <sheets>
     <sheet name="20120806" sheetId="9" r:id="rId1"/>
@@ -35,13 +35,14 @@
     <sheet name="20120924" sheetId="34" r:id="rId26"/>
     <sheet name="20121114" sheetId="35" r:id="rId27"/>
     <sheet name="20121115" sheetId="36" r:id="rId28"/>
+    <sheet name="20121116" sheetId="37" r:id="rId29"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="205">
   <si>
     <t>20:30-22:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -850,6 +851,10 @@
   </si>
   <si>
     <t>JDBC enhancement</t>
+  </si>
+  <si>
+    <t>study HSQLDB in-memory mode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2494,7 +2499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F10:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
@@ -2531,6 +2536,37 @@
       </c>
       <c r="H12" t="s">
         <v>203</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="F10:M10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="10" spans="6:13" x14ac:dyDescent="0.15">
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>204</v>
+      </c>
+      <c r="K10" t="s">
+        <v>195</v>
+      </c>
+      <c r="M10" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>